<commit_message>
Added balanced total examples
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/sentiment_balance.xlsx
+++ b/data_exploration/acl/tables/sentiment_balance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Language</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Ratio</t>
+  </si>
+  <si>
+    <t>Balanced_total</t>
   </si>
   <si>
     <t>Arabic</t>
@@ -443,13 +446,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,10 +468,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>30137</v>
@@ -482,10 +488,13 @@
       <c r="E2">
         <v>0.8408526547808376</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>11408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>290</v>
@@ -499,10 +508,13 @@
       <c r="E3">
         <v>0.5141843971631206</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>3719</v>
@@ -516,10 +528,13 @@
       <c r="E4">
         <v>0.7529864345009111</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>55</v>
@@ -533,10 +548,13 @@
       <c r="E5">
         <v>0.119047619047619</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>851</v>
@@ -550,10 +568,13 @@
       <c r="E6">
         <v>0.827016520894072</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>668</v>
@@ -567,10 +588,13 @@
       <c r="E7">
         <v>0.8466413181242078</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>970</v>
@@ -584,10 +608,13 @@
       <c r="E8">
         <v>0.7158671586715867</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>5949</v>
@@ -601,10 +628,13 @@
       <c r="E9">
         <v>0.6836359457595955</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>5506</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>93639</v>
@@ -618,10 +648,13 @@
       <c r="E10">
         <v>0.9335240810711117</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>13336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>6988</v>
@@ -635,10 +668,13 @@
       <c r="E11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>13976</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>1883</v>
@@ -652,10 +688,13 @@
       <c r="E12">
         <v>0.5817114612295335</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>165</v>
@@ -669,10 +708,13 @@
       <c r="E13">
         <v>0.3286852589641434</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1766</v>
@@ -686,10 +728,13 @@
       <c r="E14">
         <v>0.6601869158878505</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>3178</v>
@@ -703,10 +748,13 @@
       <c r="E15">
         <v>0.8533834586466166</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>3363</v>
@@ -720,10 +768,13 @@
       <c r="E16">
         <v>0.4150314698259904</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>6726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>523</v>
@@ -737,10 +788,13 @@
       <c r="E17">
         <v>0.5715846994535519</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>1186</v>
@@ -754,10 +808,13 @@
       <c r="E18">
         <v>0.4974832214765101</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>11593</v>
@@ -771,10 +828,13 @@
       <c r="E19">
         <v>0.6009226622434169</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>15398</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>26544</v>
@@ -787,6 +847,9 @@
       </c>
       <c r="E20">
         <v>0.8503059230547458</v>
+      </c>
+      <c r="F20">
+        <v>9346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>